<commit_message>
Moved imports to top of main function
</commit_message>
<xml_diff>
--- a/results/100keV_10000_simulations_results.xlsx
+++ b/results/100keV_10000_simulations_results.xlsx
@@ -454,7 +454,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>28439244</v>
+        <v>28444292</v>
       </c>
     </row>
     <row r="3">
@@ -464,7 +464,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>22255415</v>
+        <v>22247864</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2508055</v>
+        <v>2508905</v>
       </c>
     </row>
     <row r="5">
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>938735</v>
+        <v>937804</v>
       </c>
     </row>
     <row r="6">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>212261</v>
+        <v>211989</v>
       </c>
     </row>
     <row r="7">
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>171475</v>
+        <v>171674</v>
       </c>
     </row>
     <row r="8">
@@ -514,7 +514,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2111917</v>
+        <v>2114127</v>
       </c>
     </row>
     <row r="9">
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5323132</v>
+        <v>5324879</v>
       </c>
     </row>
     <row r="10">
@@ -534,7 +534,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3362909</v>
+        <v>3362109</v>
       </c>
     </row>
     <row r="11">
@@ -544,7 +544,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>320857</v>
+        <v>320394</v>
       </c>
     </row>
     <row r="12">
@@ -554,7 +554,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>140152</v>
+        <v>140506</v>
       </c>
     </row>
     <row r="13">
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>60909634</v>
+        <v>60907472</v>
       </c>
     </row>
     <row r="14">
@@ -574,7 +574,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>97794925</v>
+        <v>97798729</v>
       </c>
     </row>
     <row r="15">
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>129934507</v>
+        <v>129939633</v>
       </c>
     </row>
     <row r="16">
@@ -594,7 +594,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>156155752</v>
+        <v>156184630</v>
       </c>
     </row>
     <row r="17">
@@ -604,7 +604,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>118647203</v>
+        <v>118683194</v>
       </c>
     </row>
     <row r="18">
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>72728169</v>
+        <v>72741773</v>
       </c>
     </row>
     <row r="19">
@@ -624,7 +624,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>140387</v>
+        <v>140404</v>
       </c>
     </row>
     <row r="20">
@@ -634,7 +634,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>44521</v>
+        <v>44314</v>
       </c>
     </row>
     <row r="21">
@@ -644,7 +644,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>18835</v>
+        <v>18803</v>
       </c>
     </row>
     <row r="22">
@@ -654,7 +654,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>113739</v>
+        <v>114128</v>
       </c>
     </row>
     <row r="23">
@@ -664,7 +664,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>26062</v>
+        <v>25864</v>
       </c>
     </row>
     <row r="24">
@@ -674,7 +674,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>11373</v>
+        <v>11299</v>
       </c>
     </row>
     <row r="25">
@@ -684,7 +684,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>4419</v>
+        <v>4279</v>
       </c>
     </row>
     <row r="26">
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>176492</v>
+        <v>176586</v>
       </c>
     </row>
     <row r="27">
@@ -704,7 +704,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>5527</v>
+        <v>5320</v>
       </c>
     </row>
     <row r="28">
@@ -714,7 +714,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>10214</v>
+        <v>10390</v>
       </c>
     </row>
     <row r="29">
@@ -724,7 +724,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>5922</v>
+        <v>5900</v>
       </c>
     </row>
   </sheetData>
@@ -765,7 +765,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>358334474.4</v>
+        <v>358398079.2</v>
       </c>
     </row>
     <row r="3">
@@ -775,7 +775,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>323148625.8</v>
+        <v>323038985.28</v>
       </c>
     </row>
     <row r="4">
@@ -785,7 +785,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>38373241.5</v>
+        <v>38386246.5</v>
       </c>
     </row>
     <row r="5">
@@ -795,7 +795,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17160075.8</v>
+        <v>17143057.12</v>
       </c>
     </row>
     <row r="6">
@@ -805,7 +805,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4266446.100000001</v>
+        <v>4260978.9</v>
       </c>
     </row>
     <row r="7">
@@ -815,7 +815,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3501519.5</v>
+        <v>3505583.08</v>
       </c>
     </row>
     <row r="8">
@@ -825,7 +825,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>41541407.39</v>
+        <v>41584878.09</v>
       </c>
     </row>
     <row r="9">
@@ -835,7 +835,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>24912257.76</v>
+        <v>24920433.72</v>
       </c>
     </row>
     <row r="10">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>16646399.55</v>
+        <v>16642439.55</v>
       </c>
     </row>
     <row r="11">
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3035307.22</v>
+        <v>3030927.24</v>
       </c>
     </row>
     <row r="12">
@@ -865,7 +865,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1291722.559604453</v>
+        <v>1296114.280096082</v>
       </c>
     </row>
     <row r="13">
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>22049287.508</v>
+        <v>22048504.864</v>
       </c>
     </row>
     <row r="14">
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>18581035.75</v>
+        <v>18581758.51</v>
       </c>
     </row>
     <row r="15">
@@ -895,7 +895,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>48595505.618</v>
+        <v>48597422.742</v>
       </c>
     </row>
     <row r="16">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>25297231.824</v>
+        <v>25301910.06</v>
       </c>
     </row>
     <row r="17">
@@ -915,7 +915,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>925448.1834</v>
+        <v>925728.9132</v>
       </c>
     </row>
     <row r="18">
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>945466.1969999999</v>
+        <v>945643.049</v>
       </c>
     </row>
     <row r="19">
@@ -935,7 +935,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1431947.4</v>
+        <v>1432120.8</v>
       </c>
     </row>
     <row r="20">
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>537813.6800000001</v>
+        <v>535313.12</v>
       </c>
     </row>
     <row r="21">
@@ -955,7 +955,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>240146.25</v>
+        <v>239738.25</v>
       </c>
     </row>
     <row r="22">
@@ -965,7 +965,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>214966.71</v>
+        <v>215701.92</v>
       </c>
     </row>
     <row r="23">
@@ -975,7 +975,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>66458.09999999999</v>
+        <v>65953.2</v>
       </c>
     </row>
     <row r="24">
@@ -985,7 +985,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>32526.78</v>
+        <v>32315.14</v>
       </c>
     </row>
     <row r="25">
@@ -995,7 +995,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>13389.57</v>
+        <v>12965.37</v>
       </c>
     </row>
     <row r="26">
@@ -1005,7 +1005,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>508296.96</v>
+        <v>508567.68</v>
       </c>
     </row>
     <row r="27">
@@ -1015,7 +1015,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>35814.96</v>
+        <v>34473.60000000001</v>
       </c>
     </row>
     <row r="28">
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>76502.86</v>
+        <v>77821.10000000001</v>
       </c>
     </row>
     <row r="29">
@@ -1035,7 +1035,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>47376</v>
+        <v>47200</v>
       </c>
     </row>
   </sheetData>
@@ -1076,7 +1076,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>320857</v>
+        <v>320394</v>
       </c>
     </row>
     <row r="3">
@@ -1086,7 +1086,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>212261</v>
+        <v>211989</v>
       </c>
     </row>
     <row r="4">
@@ -1096,7 +1096,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3534384</v>
+        <v>3533783</v>
       </c>
     </row>
     <row r="5">
@@ -1106,7 +1106,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2508055</v>
+        <v>2508905</v>
       </c>
     </row>
     <row r="6">
@@ -1116,7 +1116,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6402019</v>
+        <v>6403189</v>
       </c>
     </row>
     <row r="7">
@@ -1126,7 +1126,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>22255415</v>
+        <v>22247864</v>
       </c>
     </row>
     <row r="8">
@@ -1136,7 +1136,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>28439244</v>
+        <v>28444292</v>
       </c>
     </row>
     <row r="9">
@@ -1146,7 +1146,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2111917</v>
+        <v>2114127</v>
       </c>
     </row>
     <row r="10">
@@ -1156,7 +1156,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>28111665</v>
+        <v>28105126</v>
       </c>
     </row>
     <row r="11">
@@ -1166,7 +1166,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>938735</v>
+        <v>937804</v>
       </c>
     </row>
     <row r="12">
@@ -1176,7 +1176,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>140152</v>
+        <v>140506</v>
       </c>
     </row>
     <row r="13">
@@ -1186,7 +1186,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>10627916</v>
+        <v>10631651</v>
       </c>
     </row>
     <row r="14">
@@ -1196,7 +1196,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>171475</v>
+        <v>171674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>